<commit_message>
v5.4.1: Small changed to plots and menus, beginning of larger changes to the view from inches to pixels.
</commit_message>
<xml_diff>
--- a/MVI_Information.xlsx
+++ b/MVI_Information.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnel\Documents\MATLAB\VOGA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C88D17-B3F2-40C3-92EA-4A52C804A2F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B9AAD1-3D8B-48C1-8245-FA91785A21C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="14400" windowHeight="8235" xr2:uid="{5492E525-EE99-8040-A434-353228F4B206}"/>
+    <workbookView xWindow="1170" yWindow="1500" windowWidth="16860" windowHeight="10860" xr2:uid="{5492E525-EE99-8040-A434-353228F4B206}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
   <si>
     <t>MVI001R019</t>
   </si>
@@ -66,9 +66,6 @@
     <t>MVI009R908</t>
   </si>
   <si>
-    <t>Settings Changes</t>
-  </si>
-  <si>
     <t>MVI010R141</t>
   </si>
   <si>
@@ -139,6 +136,27 @@
   </si>
   <si>
     <t>E11 (E10 until 2022-10-05)</t>
+  </si>
+  <si>
+    <t>MVI011R031</t>
+  </si>
+  <si>
+    <t>MVI012R897</t>
+  </si>
+  <si>
+    <t>MVI013R864</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Changes</t>
   </si>
 </sst>
 </file>
@@ -501,73 +519,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F4C117F-76BB-5A4B-A691-C2F0544A3D8B}">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.375" customWidth="1"/>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="9.25" customWidth="1"/>
-    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="2" max="2" width="5.125" customWidth="1"/>
+    <col min="3" max="3" width="5.5" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="9.25" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
       <c r="H1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>42594</v>
       </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="2">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="2">
         <v>42620</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="1"/>
+      <c r="I2" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -576,263 +600,357 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>42678</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
         <v>29</v>
       </c>
-      <c r="E3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="2">
         <v>42704</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="1"/>
+      <c r="I3" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>42769</v>
       </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="2">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="2">
         <v>42789</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="1"/>
+      <c r="I4" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>43084</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
         <v>29</v>
       </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="2">
         <v>43104</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="1"/>
+      <c r="I5" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>43337</v>
       </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
       <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
         <v>32</v>
       </c>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>43355</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="1"/>
+      <c r="I6" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="2">
         <v>43333</v>
       </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="2">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="2">
         <v>43369</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="2">
         <v>43479</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
         <v>29</v>
       </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="2">
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="2">
         <v>43502</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D9" s="2">
         <v>43721</v>
       </c>
-      <c r="D9" t="s">
-        <v>29</v>
-      </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="2">
+        <v>30</v>
+      </c>
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="2">
         <v>43747</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="1"/>
+      <c r="I9" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>44099</v>
       </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="2">
+        <v>31</v>
+      </c>
+      <c r="G10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="2">
         <v>44118</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="1"/>
+      <c r="I10" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D11" s="2">
         <v>44400</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="2">
+        <v>44433</v>
+      </c>
+      <c r="I11" s="2">
+        <v>44769</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>45055</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s">
         <v>29</v>
       </c>
-      <c r="E11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="2">
-        <v>44433</v>
-      </c>
-      <c r="H11" s="2">
-        <v>44769</v>
+      <c r="G12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="2">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>45079</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="2">
+        <v>45105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
+        <v>45118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v5.5.0: Useable version with proper summary plot script
</commit_message>
<xml_diff>
--- a/MVI_Information.xlsx
+++ b/MVI_Information.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnel\Documents\MATLAB\VOGA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B9AAD1-3D8B-48C1-8245-FA91785A21C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE95514-88D1-41F0-928D-5CD1FBFC36E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1500" windowWidth="16860" windowHeight="10860" xr2:uid="{5492E525-EE99-8040-A434-353228F4B206}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="14400" windowHeight="8235" xr2:uid="{5492E525-EE99-8040-A434-353228F4B206}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="44">
   <si>
     <t>MVI001R019</t>
   </si>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F4C117F-76BB-5A4B-A691-C2F0544A3D8B}">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -952,6 +952,18 @@
       <c r="D14" s="2">
         <v>45118</v>
       </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="2">
+        <v>45140</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>